<commit_message>
refresh token logic implemented
</commit_message>
<xml_diff>
--- a/DailyTaskSheet.xlsx
+++ b/DailyTaskSheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -88,6 +88,14 @@
   </si>
   <si>
     <t xml:space="preserve">1)Authentication and authorization based navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)Admin dashboard data fetch 
+2)Applying refresh token logic and handling jwt token based on it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">naman-tatvasoft/job-portal (github.com) 
+https://github.com/naman-tatvasoft/JobApplicationPortal</t>
   </si>
 </sst>
 </file>
@@ -343,10 +351,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -412,9 +420,29 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="n">
+        <v>45841</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
+        <v>45842</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="naman-tatvasoft/job-portal (github.com) "/>
+    <hyperlink ref="D5" r:id="rId2" display="naman-tatvasoft/job-portal (github.com) &#10;https://github.com/naman-tatvasoft/JobApplicationPortal"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>